<commit_message>
fix for scrapping linkedIn
</commit_message>
<xml_diff>
--- a/LoginLinkedIn/Data/courses.xlsx
+++ b/LoginLinkedIn/Data/courses.xlsx
@@ -14,7 +14,47 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <x:si>
+    <x:t>Column1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Column2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UiPath: Robotic Process Automation (RPA)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COURSE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Introducing Robotic Process Automation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RPA: Automation Anywhere</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RPA, AI, and Cognitive Tech for Leaders</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UiPath Essential Training</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RPA: Automation Anywhere IQ Bot</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Robotic Process Automation: Tech Primer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Blue Prism: Excel Automation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Introducing Blue Prism</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Digital Technologies Case Studies: AI, IOT, Robotics, Blockchain</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -368,7 +408,96 @@
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData/>
+  <x:sheetData>
+    <x:row r="1" spans="1:2">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:2">
+      <x:c r="A2" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:2">
+      <x:c r="A3" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:2">
+      <x:c r="A4" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:2">
+      <x:c r="A5" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:2">
+      <x:c r="A6" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:2">
+      <x:c r="A7" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:2">
+      <x:c r="A8" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:2">
+      <x:c r="A9" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:2">
+      <x:c r="A10" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:2">
+      <x:c r="A11" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>

</xml_diff>